<commit_message>
feat(video): increase view count on video detail page
</commit_message>
<xml_diff>
--- a/TatCaChucNang_DAO_Controller_JSP.xlsx
+++ b/TatCaChucNang_DAO_Controller_JSP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,46 +95,46 @@
     <t>FavoriteServlet</t>
   </si>
   <si>
+    <t>Unlike video</t>
+  </si>
+  <si>
+    <t>void unlike(String userId, String videoId)</t>
+  </si>
+  <si>
+    <t>Danh sách video yêu thích</t>
+  </si>
+  <si>
+    <t>List&lt;Video&gt; findFavoritesByUser(String userId)</t>
+  </si>
+  <si>
+    <t>favorites.jsp</t>
+  </si>
+  <si>
+    <t>Tăng views khi nhấn vào xem chi tiết video</t>
+  </si>
+  <si>
+    <t>void saveViewHistory(String userId, String videoId)</t>
+  </si>
+  <si>
+    <t>HistoryServlet</t>
+  </si>
+  <si>
+    <t>history.jsp</t>
+  </si>
+  <si>
+    <t>Nhập email để chia sẻ video</t>
+  </si>
+  <si>
+    <t>void share(String userId, String videoId, String emails)</t>
+  </si>
+  <si>
+    <t>ShareServlet</t>
+  </si>
+  <si>
+    <t>share.jsp</t>
+  </si>
+  <si>
     <t>Chưa xong</t>
-  </si>
-  <si>
-    <t>Unlike video</t>
-  </si>
-  <si>
-    <t>void unlike(String userId, String videoId)</t>
-  </si>
-  <si>
-    <t>Danh sách video yêu thích</t>
-  </si>
-  <si>
-    <t>List&lt;Video&gt; findFavoritesByUser(String userId)</t>
-  </si>
-  <si>
-    <t>favorites.jsp</t>
-  </si>
-  <si>
-    <t>Ghi nhận video đã xem qua cookie/session</t>
-  </si>
-  <si>
-    <t>void saveViewHistory(String userId, String videoId)</t>
-  </si>
-  <si>
-    <t>HistoryServlet</t>
-  </si>
-  <si>
-    <t>history.jsp</t>
-  </si>
-  <si>
-    <t>Nhập email để chia sẻ video</t>
-  </si>
-  <si>
-    <t>void share(String userId, String videoId, String emails)</t>
-  </si>
-  <si>
-    <t>ShareServlet</t>
-  </si>
-  <si>
-    <t>share.jsp</t>
   </si>
   <si>
     <t>Gửi link video qua email</t>
@@ -1398,8 +1398,8 @@
   <sheetPr/>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1529,7 +1529,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1537,10 +1537,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1549,7 +1549,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1557,19 +1557,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1577,19 +1577,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1597,19 +1597,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1623,13 +1623,13 @@
         <v>37</v>
       </c>
       <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1643,13 +1643,13 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1669,7 +1669,7 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1689,7 +1689,7 @@
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1709,7 +1709,7 @@
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1729,7 +1729,7 @@
         <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1749,7 +1749,7 @@
         <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1769,7 +1769,7 @@
         <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1789,7 +1789,7 @@
         <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1809,7 +1809,7 @@
         <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1829,7 +1829,7 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1849,7 +1849,7 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1869,7 +1869,7 @@
         <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1889,7 +1889,7 @@
         <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1909,7 +1909,7 @@
         <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1929,7 +1929,7 @@
         <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1949,7 +1949,7 @@
         <v>81</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1969,7 +1969,7 @@
         <v>84</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1989,7 +1989,7 @@
         <v>87</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2009,7 +2009,7 @@
         <v>91</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2029,7 +2029,7 @@
         <v>91</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2049,7 +2049,7 @@
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2069,7 +2069,7 @@
         <v>91</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2089,7 +2089,7 @@
         <v>91</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2109,7 +2109,7 @@
         <v>91</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2129,7 +2129,7 @@
         <v>91</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2149,7 +2149,7 @@
         <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2169,7 +2169,7 @@
         <v>115</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2189,7 +2189,7 @@
         <v>118</v>
       </c>
       <c r="F39" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2209,7 +2209,7 @@
         <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2223,13 +2223,13 @@
         <v>122</v>
       </c>
       <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" t="s">
         <v>30</v>
       </c>
-      <c r="E41" t="s">
-        <v>31</v>
-      </c>
       <c r="F41" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2249,7 +2249,7 @@
         <v>126</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: Share video via email functionality + share form
</commit_message>
<xml_diff>
--- a/TatCaChucNang_DAO_Controller_JSP.xlsx
+++ b/TatCaChucNang_DAO_Controller_JSP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8400"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
   <si>
     <t>STT</t>
   </si>
@@ -47,6 +47,9 @@
     <t>Hoàn thành</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
     <t>Hiển thị 6 video nhiều lượt xem nhất</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
     <t>Đã hoàn thành</t>
   </si>
   <si>
+    <t>user</t>
+  </si>
+  <si>
     <t>Hiển thị 6 video mới nhất</t>
   </si>
   <si>
@@ -134,33 +140,21 @@
     <t>share.jsp</t>
   </si>
   <si>
+    <t>Đăng ký tài khoản (gửi mail chào mừng)</t>
+  </si>
+  <si>
+    <t>void register(User user)</t>
+  </si>
+  <si>
+    <t>UserServlet</t>
+  </si>
+  <si>
+    <t>register.jsp</t>
+  </si>
+  <si>
     <t>Chưa xong</t>
   </si>
   <si>
-    <t>Gửi link video qua email</t>
-  </si>
-  <si>
-    <t>void sendMail(Share share)</t>
-  </si>
-  <si>
-    <t>Tự động lưu thời gian chia sẻ (share_date)</t>
-  </si>
-  <si>
-    <t>share.setShareDate(new Date())</t>
-  </si>
-  <si>
-    <t>Đăng ký tài khoản (gửi mail chào mừng)</t>
-  </si>
-  <si>
-    <t>void register(User user)</t>
-  </si>
-  <si>
-    <t>UserServlet</t>
-  </si>
-  <si>
-    <t>register.jsp</t>
-  </si>
-  <si>
     <t>Đăng nhập / đăng xuất</t>
   </si>
   <si>
@@ -384,12 +378,6 @@
   </si>
   <si>
     <t>tất cả file JSP</t>
-  </si>
-  <si>
-    <t>Hiển thị video từ link YouTube bằng iframe</t>
-  </si>
-  <si>
-    <t>iframe + link</t>
   </si>
   <si>
     <t>Lưu lịch sử xem video</t>
@@ -1396,23 +1384,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="4.66666666666667" customWidth="1"/>
-    <col min="2" max="2" width="47.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="60.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="19.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="45.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="55.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="17.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="19.7777777777778" customWidth="1"/>
-    <col min="6" max="6" width="11.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,830 +1419,800 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
       <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="s">
-        <v>61</v>
-      </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" t="s">
-        <v>72</v>
-      </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D38" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="E38" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" t="s">
-        <v>29</v>
-      </c>
-      <c r="E41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" t="s">
-        <v>125</v>
-      </c>
-      <c r="E42" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10 F11:F37 F38:F39">
       <formula1>"Chưa xong,Đã hoàn thành"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>